<commit_message>
Add additional CI columns to TableAUC tables
</commit_message>
<xml_diff>
--- a/figures/ssGSEA_TableAUC.xlsx
+++ b/figures/ssGSEA_TableAUC.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aubre\Documents\BU Research\tbsp_malnutrition\figures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94944072-460C-46CC-AA18-95B0EB494DC9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11853D9A-C750-4947-9A5D-CE3A64D7892D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
   <si>
     <t>Signature</t>
   </si>
@@ -173,6 +173,12 @@
   </si>
   <si>
     <t>Gjoen_7</t>
+  </si>
+  <si>
+    <t>LowerCISunXu</t>
+  </si>
+  <si>
+    <t>UpperCISunXu</t>
   </si>
 </sst>
 </file>
@@ -661,11 +667,14 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1021,38 +1030,50 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F47"/>
+  <dimension ref="A1:H47"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="131" workbookViewId="0">
-      <selection activeCell="A43" sqref="A43"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="18.26953125" customWidth="1"/>
+    <col min="3" max="3" width="17" customWidth="1"/>
+    <col min="4" max="4" width="9.7265625" customWidth="1"/>
+    <col min="5" max="5" width="6.90625" customWidth="1"/>
+    <col min="6" max="6" width="10.90625" customWidth="1"/>
+    <col min="7" max="7" width="12.81640625" customWidth="1"/>
+    <col min="8" max="8" width="12.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
+    <row r="1" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G1" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -1071,8 +1092,14 @@
       <c r="F2" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G2" s="2">
+        <v>0.96703708129600596</v>
+      </c>
+      <c r="H2" s="2">
+        <v>0.98863636363636398</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>39</v>
       </c>
@@ -1091,8 +1118,14 @@
       <c r="F3" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G3" s="2">
+        <v>0.94773891861905901</v>
+      </c>
+      <c r="H3" s="2">
+        <v>0.98295454545454497</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -1111,8 +1144,14 @@
       <c r="F4" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G4" s="2">
+        <v>0.93126722502248505</v>
+      </c>
+      <c r="H4" s="2">
+        <v>0.97727272727272696</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>43</v>
       </c>
@@ -1131,8 +1170,14 @@
       <c r="F5" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G5" s="2">
+        <v>0.92617971798033905</v>
+      </c>
+      <c r="H5" s="2">
+        <v>0.97159090909090895</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>32</v>
       </c>
@@ -1151,8 +1196,14 @@
       <c r="F6" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G6" s="2">
+        <v>0.91555891352403196</v>
+      </c>
+      <c r="H6" s="2">
+        <v>0.96875</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>50</v>
       </c>
@@ -1171,8 +1222,14 @@
       <c r="F7" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G7" s="2">
+        <v>0.91658326294811598</v>
+      </c>
+      <c r="H7" s="2">
+        <v>0.96590909090909105</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -1191,8 +1248,14 @@
       <c r="F8" s="2">
         <v>0.99460000000000004</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G8" s="2">
+        <v>0.91470351430631403</v>
+      </c>
+      <c r="H8" s="2">
+        <v>0.96590909090909105</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>42</v>
       </c>
@@ -1211,8 +1274,14 @@
       <c r="F9" s="2">
         <v>0.99729999999999996</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G9" s="2">
+        <v>0.91922821903416996</v>
+      </c>
+      <c r="H9" s="2">
+        <v>0.96590909090909105</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -1231,8 +1300,14 @@
       <c r="F10" s="2">
         <v>0.99739999999999995</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G10" s="2">
+        <v>0.91333102494881602</v>
+      </c>
+      <c r="H10" s="2">
+        <v>0.96306818181818199</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>33</v>
       </c>
@@ -1251,8 +1326,14 @@
       <c r="F11" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G11" s="2">
+        <v>0.90517577996444798</v>
+      </c>
+      <c r="H11" s="2">
+        <v>0.96022727272727304</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>45</v>
       </c>
@@ -1271,8 +1352,14 @@
       <c r="F12" s="2">
         <v>0.99080000000000001</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G12" s="2">
+        <v>0.90249063422686004</v>
+      </c>
+      <c r="H12" s="2">
+        <v>0.95738636363636398</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -1291,8 +1378,14 @@
       <c r="F13" s="2">
         <v>0.99109999999999998</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G13" s="2">
+        <v>0.88090215038608899</v>
+      </c>
+      <c r="H13" s="2">
+        <v>0.94602272727272696</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>16</v>
       </c>
@@ -1311,8 +1404,14 @@
       <c r="F14" s="2">
         <v>0.98629999999999995</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G14" s="2">
+        <v>0.87286804791819195</v>
+      </c>
+      <c r="H14" s="2">
+        <v>0.94318181818181801</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>48</v>
       </c>
@@ -1331,8 +1430,14 @@
       <c r="F15" s="2">
         <v>0.98860000000000003</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G15" s="2">
+        <v>0.87212016694806305</v>
+      </c>
+      <c r="H15" s="2">
+        <v>0.94034090909090895</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>38</v>
       </c>
@@ -1351,8 +1456,14 @@
       <c r="F16" s="2">
         <v>0.98319999999999996</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G16" s="2">
+        <v>0.86841477141568102</v>
+      </c>
+      <c r="H16" s="2">
+        <v>0.9375</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>31</v>
       </c>
@@ -1371,8 +1482,14 @@
       <c r="F17" s="2">
         <v>0.98809999999999998</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G17" s="2">
+        <v>0.84744358064512804</v>
+      </c>
+      <c r="H17" s="2">
+        <v>0.92897727272727304</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>13</v>
       </c>
@@ -1391,8 +1508,14 @@
       <c r="F18" s="2">
         <v>0.98260000000000003</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G18" s="2">
+        <v>0.84910535419679301</v>
+      </c>
+      <c r="H18" s="2">
+        <v>0.92613636363636398</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>23</v>
       </c>
@@ -1411,8 +1534,14 @@
       <c r="F19" s="2">
         <v>0.97770000000000001</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G19" s="2">
+        <v>0.831021247038912</v>
+      </c>
+      <c r="H19" s="2">
+        <v>0.92045454545454497</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>30</v>
       </c>
@@ -1431,8 +1560,14 @@
       <c r="F20" s="2">
         <v>0.98619999999999997</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G20" s="2">
+        <v>0.80994590681570899</v>
+      </c>
+      <c r="H20" s="2">
+        <v>0.90625</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>14</v>
       </c>
@@ -1451,8 +1586,14 @@
       <c r="F21" s="2">
         <v>0.97170000000000001</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G21" s="2">
+        <v>0.78122322107984998</v>
+      </c>
+      <c r="H21" s="2">
+        <v>0.89488636363636398</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>18</v>
       </c>
@@ -1471,8 +1612,14 @@
       <c r="F22" s="2">
         <v>0.96689999999999998</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G22" s="2">
+        <v>0.78356604995389401</v>
+      </c>
+      <c r="H22" s="2">
+        <v>0.88920454545454497</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>8</v>
       </c>
@@ -1491,8 +1638,14 @@
       <c r="F23" s="2">
         <v>0.95830000000000004</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G23" s="2">
+        <v>0.78409097024402497</v>
+      </c>
+      <c r="H23" s="2">
+        <v>0.88636363636363602</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>7</v>
       </c>
@@ -1511,8 +1664,14 @@
       <c r="F24" s="2">
         <v>0.9617</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G24" s="2">
+        <v>0.779296822968225</v>
+      </c>
+      <c r="H24" s="2">
+        <v>0.88352272727272696</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>28</v>
       </c>
@@ -1531,8 +1690,14 @@
       <c r="F25" s="2">
         <v>0.9556</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G25" s="2">
+        <v>0.75601360219948199</v>
+      </c>
+      <c r="H25" s="2">
+        <v>0.87215909090909105</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>34</v>
       </c>
@@ -1551,8 +1716,14 @@
       <c r="F26" s="2">
         <v>0.95830000000000004</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G26" s="2">
+        <v>0.73670988507617696</v>
+      </c>
+      <c r="H26" s="2">
+        <v>0.86079545454545503</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>22</v>
       </c>
@@ -1571,8 +1742,14 @@
       <c r="F27" s="2">
         <v>0.93669999999999998</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G27" s="2">
+        <v>0.73395860258469803</v>
+      </c>
+      <c r="H27" s="2">
+        <v>0.85227272727272696</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>49</v>
       </c>
@@ -1591,8 +1768,14 @@
       <c r="F28" s="2">
         <v>0.9425</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G28" s="2">
+        <v>0.72915000819590303</v>
+      </c>
+      <c r="H28" s="2">
+        <v>0.84943181818181801</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>44</v>
       </c>
@@ -1611,8 +1794,14 @@
       <c r="F29" s="2">
         <v>0.92059999999999997</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G29" s="2">
+        <v>0.72240747039615305</v>
+      </c>
+      <c r="H29" s="2">
+        <v>0.84375</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>17</v>
       </c>
@@ -1631,8 +1820,14 @@
       <c r="F30" s="2">
         <v>0.92620000000000002</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G30" s="2">
+        <v>0.71383991960457505</v>
+      </c>
+      <c r="H30" s="2">
+        <v>0.83806818181818199</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>20</v>
       </c>
@@ -1651,8 +1846,14 @@
       <c r="F31" s="2">
         <v>0.93620000000000003</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G31" s="2">
+        <v>0.71225281688962605</v>
+      </c>
+      <c r="H31" s="2">
+        <v>0.83806818181818199</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>15</v>
       </c>
@@ -1671,8 +1872,14 @@
       <c r="F32" s="2">
         <v>0.91920000000000002</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G32" s="2">
+        <v>0.70428519974447701</v>
+      </c>
+      <c r="H32" s="2">
+        <v>0.83522727272727304</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>36</v>
       </c>
@@ -1691,8 +1898,14 @@
       <c r="F33" s="2">
         <v>0.91739999999999999</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G33" s="2">
+        <v>0.69741811748195803</v>
+      </c>
+      <c r="H33" s="2">
+        <v>0.82954545454545503</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>9</v>
       </c>
@@ -1711,8 +1924,14 @@
       <c r="F34" s="2">
         <v>0.9405</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G34" s="2">
+        <v>0.68613744132913002</v>
+      </c>
+      <c r="H34" s="2">
+        <v>0.82102272727272696</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>41</v>
       </c>
@@ -1731,8 +1950,14 @@
       <c r="F35" s="2">
         <v>0.91069999999999995</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G35" s="2">
+        <v>0.65605827995773103</v>
+      </c>
+      <c r="H35" s="2">
+        <v>0.79829545454545503</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>40</v>
       </c>
@@ -1751,8 +1976,14 @@
       <c r="F36" s="2">
         <v>0.89019999999999999</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G36" s="2">
+        <v>0.64216787003992204</v>
+      </c>
+      <c r="H36" s="2">
+        <v>0.78693181818181801</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>47</v>
       </c>
@@ -1771,8 +2002,14 @@
       <c r="F37" s="2">
         <v>0.89739999999999998</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G37" s="2">
+        <v>0.62386647586039001</v>
+      </c>
+      <c r="H37" s="2">
+        <v>0.77272727272727304</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>46</v>
       </c>
@@ -1791,8 +2028,14 @@
       <c r="F38" s="2">
         <v>0.9022</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G38" s="2">
+        <v>0.60187985947063705</v>
+      </c>
+      <c r="H38" s="2">
+        <v>0.76988636363636398</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>25</v>
       </c>
@@ -1811,8 +2054,14 @@
       <c r="F39" s="2">
         <v>0.84319999999999995</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G39" s="2">
+        <v>0.56380644156330095</v>
+      </c>
+      <c r="H39" s="2">
+        <v>0.73011363636363602</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>26</v>
       </c>
@@ -1831,8 +2080,14 @@
       <c r="F40" s="2">
         <v>0.85729999999999995</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G40" s="2">
+        <v>0.54623943578998801</v>
+      </c>
+      <c r="H40" s="2">
+        <v>0.71590909090909105</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>6</v>
       </c>
@@ -1851,8 +2106,14 @@
       <c r="F41" s="2">
         <v>0.77949999999999997</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G41" s="2">
+        <v>0.48193798095135498</v>
+      </c>
+      <c r="H41" s="2">
+        <v>0.66193181818181801</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>37</v>
       </c>
@@ -1871,8 +2132,14 @@
       <c r="F42" s="2">
         <v>0.81410000000000005</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G42" s="2">
+        <v>0.48566764254681699</v>
+      </c>
+      <c r="H42" s="2">
+        <v>0.66193181818181801</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>29</v>
       </c>
@@ -1891,8 +2158,14 @@
       <c r="F43" s="2">
         <v>0.75700000000000001</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G43" s="2">
+        <v>0.42079728301720898</v>
+      </c>
+      <c r="H43" s="2">
+        <v>0.61079545454545503</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>35</v>
       </c>
@@ -1911,8 +2184,14 @@
       <c r="F44" s="2">
         <v>0.74380000000000002</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G44" s="2">
+        <v>0.4213244335886</v>
+      </c>
+      <c r="H44" s="2">
+        <v>0.60511363636363602</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>27</v>
       </c>
@@ -1931,8 +2210,14 @@
       <c r="F45" s="2">
         <v>0.75670000000000004</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G45" s="2">
+        <v>0.37610017877262097</v>
+      </c>
+      <c r="H45" s="2">
+        <v>0.57954545454545503</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>24</v>
       </c>
@@ -1951,8 +2236,14 @@
       <c r="F46" s="2">
         <v>0.69489999999999996</v>
       </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G46" s="2">
+        <v>0.32154115660655902</v>
+      </c>
+      <c r="H46" s="2">
+        <v>0.51136363636363602</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
       <c r="D47" s="2"/>
       <c r="E47" s="2"/>
       <c r="F47" s="2"/>

</xml_diff>